<commit_message>
Update Bugs and Build Settings
-Updated the bug sheet.
-Added the other scenes to the build settings.
</commit_message>
<xml_diff>
--- a/GSP362_TeamA_BugTracking.xlsx
+++ b/GSP362_TeamA_BugTracking.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="105" windowWidth="12435" windowHeight="6210"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
   <si>
     <t>BUG NAME</t>
   </si>
@@ -100,6 +100,18 @@
   </si>
   <si>
     <t>Removed the player acceptance loop, as it prevented the game from reaching update, which would end up freezing the game</t>
+  </si>
+  <si>
+    <t>Added collision the the map prefab and functionality to make the game end upon this collision.</t>
+  </si>
+  <si>
+    <t>Added support for passing number of players from the menu to the game scene.</t>
+  </si>
+  <si>
+    <t>Resources are editor only.</t>
+  </si>
+  <si>
+    <t>Resources are loaded with editor functions. This isn't allowed in a built game.</t>
   </si>
 </sst>
 </file>
@@ -649,7 +661,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,7 +758,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
@@ -754,14 +766,16 @@
         <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E6" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
@@ -769,12 +783,14 @@
         <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -791,11 +807,19 @@
       </c>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>